<commit_message>
added a new endpoint for greenpoints' aggregates
</commit_message>
<xml_diff>
--- a/WebApi/Database/Data/GreenScorePredictor.xlsx
+++ b/WebApi/Database/Data/GreenScorePredictor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag4488\Documents\Visual Studio 2019\Projects\Hackathon2021\FinESG_CoGoApp\WebApi\Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44BD07A0-ADD0-48A5-B60A-B70063B3ECE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7719A43D-382B-4B80-B98E-3FBA1DA45316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23670" yWindow="2655" windowWidth="24315" windowHeight="12225" xr2:uid="{10E8C4BC-9253-4B38-BAC4-2827BC92D375}"/>
+    <workbookView xWindow="-20460" yWindow="3930" windowWidth="8280" windowHeight="5625" xr2:uid="{10E8C4BC-9253-4B38-BAC4-2827BC92D375}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Points Trendline" sheetId="1" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>